<commit_message>
remove old comments, ignore some files
</commit_message>
<xml_diff>
--- a/test/excel/06000.xlsx
+++ b/test/excel/06000.xlsx
@@ -5,15 +5,15 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jeltedirks/WebstormProjects/bodyblock-conversion/static/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jeltedirks/WebstormProjects/bodyblock-conversion/test/excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2D1EAC4-3D4B-0E4A-B7D8-DC3E2C585C4B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{270EB7D4-BD72-F546-A346-C14EA6A16FAA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2200" yWindow="2560" windowWidth="22900" windowHeight="17000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="24280" yWindow="6700" windowWidth="22900" windowHeight="17000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="blad1" sheetId="1" r:id="rId1"/>
+    <sheet name="06020" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -25,7 +25,53 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+  <si>
+    <t>Eigen risico</t>
+  </si>
+  <si>
+    <t>€ 10043</t>
+  </si>
+  <si>
+    <t>06 Eigen risico               € 10043</t>
+  </si>
+  <si>
+    <t>x</t>
+  </si>
+  <si>
+    <t>10043</t>
+  </si>
+  <si>
+    <t>Getal inclusief decimalen</t>
+  </si>
+  <si>
+    <t>Links</t>
+  </si>
+  <si>
+    <t>verwijderen</t>
+  </si>
+  <si>
+    <t>omschrijving</t>
+  </si>
+  <si>
+    <t>inhoud</t>
+  </si>
+  <si>
+    <t>weergave</t>
+  </si>
+  <si>
+    <t>uitlijnen</t>
+  </si>
+  <si>
+    <t>regel verwijderen</t>
+  </si>
+  <si>
+    <t>regel template</t>
+  </si>
+  <si>
+    <t>PTEST</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -59,11 +105,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment textRotation="45"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standaard" xfId="0" builtinId="0"/>
@@ -344,10 +387,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G1"/>
+  <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G15" sqref="G15"/>
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -360,13 +403,55 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A1" s="1"/>
-      <c r="B1" s="1"/>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1"/>
-      <c r="F1" s="1"/>
-      <c r="G1" s="1"/>
+      <c r="A1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F1" t="s">
+        <v>13</v>
+      </c>
+      <c r="G1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
+        <v>1</v>
+      </c>
+      <c r="F2" t="s">
+        <v>2</v>
+      </c>
+      <c r="G2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D3" t="s">
+        <v>6</v>
+      </c>
+      <c r="E3" t="s">
+        <v>7</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
start checking for label range at next row, saves initial value to compare against. doesn't increase r with new range at the end
</commit_message>
<xml_diff>
--- a/test/excel/06000.xlsx
+++ b/test/excel/06000.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jeltedirks/WebstormProjects/bodyblock-conversion/test/excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{270EB7D4-BD72-F546-A346-C14EA6A16FAA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD21917E-3682-B442-9D12-F0D882647193}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="24280" yWindow="6700" windowWidth="22900" windowHeight="17000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4300" yWindow="6700" windowWidth="42880" windowHeight="17000" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="06020" sheetId="1" r:id="rId1"/>
+    <sheet name="02030" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="18">
   <si>
     <t>Eigen risico</t>
   </si>
@@ -70,16 +71,32 @@
   </si>
   <si>
     <t>PTEST</t>
+  </si>
+  <si>
+    <t>Verzekerd bedrag accessoires</t>
+  </si>
+  <si>
+    <t>09 Verzekerd bedrag accessoires € 11239</t>
+  </si>
+  <si>
+    <t>Rechts</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -105,8 +122,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standaard" xfId="0" builtinId="0"/>
@@ -389,7 +408,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
@@ -457,4 +476,85 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9A88B528-13D3-1344-9365-7B8862D90829}">
+  <dimension ref="A1:G3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E6" sqref="E6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="25.6640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="28" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="22.6640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.83203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.5" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="51" style="2" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="6.1640625" style="2" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+      <c r="A2" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B2" s="1">
+        <v>11239</v>
+      </c>
+      <c r="C2" s="1"/>
+      <c r="D2" s="1"/>
+      <c r="E2" s="1"/>
+      <c r="F2" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+      <c r="A3" s="1"/>
+      <c r="B3" s="1">
+        <v>11239</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F3" s="1"/>
+      <c r="G3" s="1"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
saved proper test file
</commit_message>
<xml_diff>
--- a/test/excel/06000.xlsx
+++ b/test/excel/06000.xlsx
@@ -8,13 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jeltedirks/WebstormProjects/bodyblock-conversion/test/excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD21917E-3682-B442-9D12-F0D882647193}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3613519-A596-2147-9B34-4AC7A3C87BE9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4300" yWindow="6700" windowWidth="42880" windowHeight="17000" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="2760" windowWidth="33600" windowHeight="17000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="06020" sheetId="1" r:id="rId1"/>
-    <sheet name="02030" sheetId="2" r:id="rId2"/>
+    <sheet name="02030" sheetId="2" r:id="rId1"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -26,29 +25,14 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="18">
-  <si>
-    <t>Eigen risico</t>
-  </si>
-  <si>
-    <t>€ 10043</t>
-  </si>
-  <si>
-    <t>06 Eigen risico               € 10043</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t>x</t>
   </si>
   <si>
-    <t>10043</t>
-  </si>
-  <si>
     <t>Getal inclusief decimalen</t>
   </si>
   <si>
-    <t>Links</t>
-  </si>
-  <si>
     <t>verwijderen</t>
   </si>
   <si>
@@ -80,6 +64,9 @@
   </si>
   <si>
     <t>Rechts</t>
+  </si>
+  <si>
+    <t>€ 11239</t>
   </si>
 </sst>
 </file>
@@ -405,85 +392,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G3"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="14.5" customWidth="1"/>
-    <col min="2" max="2" width="32.33203125" customWidth="1"/>
-    <col min="3" max="3" width="16.33203125" customWidth="1"/>
-    <col min="4" max="7" width="14.5" customWidth="1"/>
-    <col min="8" max="8" width="18" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C1" t="s">
-        <v>10</v>
-      </c>
-      <c r="D1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E1" t="s">
-        <v>12</v>
-      </c>
-      <c r="F1" t="s">
-        <v>13</v>
-      </c>
-      <c r="G1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" t="s">
-        <v>1</v>
-      </c>
-      <c r="F2" t="s">
-        <v>2</v>
-      </c>
-      <c r="G2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="B3" t="s">
-        <v>4</v>
-      </c>
-      <c r="C3" t="s">
-        <v>5</v>
-      </c>
-      <c r="D3" t="s">
-        <v>6</v>
-      </c>
-      <c r="E3" t="s">
-        <v>7</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9A88B528-13D3-1344-9365-7B8862D90829}">
   <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -499,42 +412,42 @@
   <sheetData>
     <row r="1" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>9</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="2" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="B2" s="1">
-        <v>11239</v>
+        <v>10</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>13</v>
       </c>
       <c r="C2" s="1"/>
       <c r="D2" s="1"/>
       <c r="E2" s="1"/>
       <c r="F2" s="1" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="16" x14ac:dyDescent="0.2">
@@ -543,18 +456,21 @@
         <v>11239</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="F3" s="1"/>
       <c r="G3" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <ignoredErrors>
+    <ignoredError sqref="B2" numberStoredAsText="1"/>
+  </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
set x in maatschappij column if subinfo has been added
</commit_message>
<xml_diff>
--- a/test/excel/06000.xlsx
+++ b/test/excel/06000.xlsx
@@ -8,12 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jeltedirks/WebstormProjects/bodyblock-conversion/test/excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3613519-A596-2147-9B34-4AC7A3C87BE9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{121E0254-E0D8-3141-A0AE-E493FDA49407}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="2760" windowWidth="33600" windowHeight="17000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="02030" sheetId="2" r:id="rId1"/>
+    <sheet name="blad1" sheetId="2" r:id="rId1"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -25,65 +25,15 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
-  <si>
-    <t>x</t>
-  </si>
-  <si>
-    <t>Getal inclusief decimalen</t>
-  </si>
-  <si>
-    <t>verwijderen</t>
-  </si>
-  <si>
-    <t>omschrijving</t>
-  </si>
-  <si>
-    <t>inhoud</t>
-  </si>
-  <si>
-    <t>weergave</t>
-  </si>
-  <si>
-    <t>uitlijnen</t>
-  </si>
-  <si>
-    <t>regel verwijderen</t>
-  </si>
-  <si>
-    <t>regel template</t>
-  </si>
-  <si>
-    <t>PTEST</t>
-  </si>
-  <si>
-    <t>Verzekerd bedrag accessoires</t>
-  </si>
-  <si>
-    <t>09 Verzekerd bedrag accessoires € 11239</t>
-  </si>
-  <si>
-    <t>Rechts</t>
-  </si>
-  <si>
-    <t>€ 11239</t>
-  </si>
-</sst>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -109,9 +59,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
@@ -393,84 +342,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9A88B528-13D3-1344-9365-7B8862D90829}">
-  <dimension ref="A1:G3"/>
+  <dimension ref="A1:G1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="25.6640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="28" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="22.6640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="7.83203125" style="2" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.5" style="2" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="51" style="2" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="6.1640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="25.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="28" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="22.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.83203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="51" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="6.1640625" style="1" bestFit="1" customWidth="1"/>
   </cols>
-  <sheetData>
-    <row r="1" spans="1:7" ht="16" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" ht="16" x14ac:dyDescent="0.2">
-      <c r="A2" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="C2" s="1"/>
-      <c r="D2" s="1"/>
-      <c r="E2" s="1"/>
-      <c r="F2" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" ht="16" x14ac:dyDescent="0.2">
-      <c r="A3" s="1"/>
-      <c r="B3" s="1">
-        <v>11239</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="F3" s="1"/>
-      <c r="G3" s="1"/>
-    </row>
-  </sheetData>
+  <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <ignoredErrors>
-    <ignoredError sqref="B2" numberStoredAsText="1"/>
-  </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>